<commit_message>
Made Changes According to Review
</commit_message>
<xml_diff>
--- a/Documentation/Lakshya_Project_Plan.xlsx
+++ b/Documentation/Lakshya_Project_Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakshya.sharma\Desktop\Reskilling\5_Azure\Project_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakshya.sharma\Desktop\Reskilling\5_Azure\Project_2\azure-ci-cd\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632C1B20-E008-4D9A-930D-5F82550A2ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101DFAB3-2095-4E2A-AB7C-A1C5ABB5E27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Start Date</t>
   </si>
@@ -67,6 +67,66 @@
   </si>
   <si>
     <t>Documentation</t>
+  </si>
+  <si>
+    <t>Quaterly Plan</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Proposed Difficulty</t>
+  </si>
+  <si>
+    <t>Feature Category</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Prepare for Project resources &amp; team allocation</t>
+  </si>
+  <si>
+    <t>Project Initialization</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Design a Model to give predictions, and link it to API</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t>Improve Quality Assurance</t>
+  </si>
+  <si>
+    <t>Implement CI CD for the project</t>
+  </si>
+  <si>
+    <t>CI/CD</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>To Do</t>
   </si>
 </sst>
 </file>
@@ -74,9 +134,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,8 +151,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +176,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -133,12 +213,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -420,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -431,9 +514,11 @@
     <col min="2" max="2" width="13.26953125" customWidth="1"/>
     <col min="3" max="3" width="45.36328125" customWidth="1"/>
     <col min="4" max="4" width="16.6328125" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -444,7 +529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>44743</v>
       </c>
@@ -455,7 +540,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>44743</v>
       </c>
@@ -466,7 +551,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>44743</v>
       </c>
@@ -477,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
         <v>44743</v>
       </c>
@@ -488,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>44743</v>
       </c>
@@ -499,7 +584,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>44743</v>
       </c>
@@ -510,7 +595,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>44743</v>
       </c>
@@ -521,7 +606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>44744</v>
       </c>
@@ -532,7 +617,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <v>44744</v>
       </c>
@@ -543,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
         <v>44744</v>
       </c>
@@ -554,7 +639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>44744</v>
       </c>
@@ -565,7 +650,93 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>